<commit_message>
Finish Report. Minor ERD changes
</commit_message>
<xml_diff>
--- a/VectorData/Description of the Log Files.xlsx
+++ b/VectorData/Description of the Log Files.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\chcfs02pi\home$\ShangA\Documents\Signal Strength Research\Ara Database Project\Example Log Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\OneDrive - Ara Institute of Canterbury\Year 2\Semester 1\Database\Assignment1\VectorData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_BEEA672BDE4C896725B57A41FD311DAD35C6B5EE" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{94B42520-F101-48FB-AEF7-457495D4F63D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -485,7 +486,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -837,17 +838,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="92.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="109.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Final Touches. Proof-reading required
</commit_message>
<xml_diff>
--- a/VectorData/Description of the Log Files.xlsx
+++ b/VectorData/Description of the Log Files.xlsx
@@ -841,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>